<commit_message>
V2.1_Beta released: --update stopwords corpus
</commit_message>
<xml_diff>
--- a/analysis/hotwords/DM.xlsx
+++ b/analysis/hotwords/DM.xlsx
@@ -31,18 +31,9 @@
     <t>经验</t>
   </si>
   <si>
-    <t>熟悉</t>
-  </si>
-  <si>
     <t>优先</t>
   </si>
   <si>
-    <t>相关</t>
-  </si>
-  <si>
-    <t>用户</t>
-  </si>
-  <si>
     <t>分析</t>
   </si>
   <si>
@@ -64,9 +55,6 @@
     <t>Python</t>
   </si>
   <si>
-    <t>工作</t>
-  </si>
-  <si>
     <t>以上学历</t>
   </si>
   <si>
@@ -76,9 +64,6 @@
     <t>开发</t>
   </si>
   <si>
-    <t>负责</t>
-  </si>
-  <si>
     <t>海量</t>
   </si>
   <si>
@@ -104,6 +89,21 @@
   </si>
   <si>
     <t>熟练掌握</t>
+  </si>
+  <si>
+    <t>数学</t>
+  </si>
+  <si>
+    <t>要求</t>
+  </si>
+  <si>
+    <t>平台</t>
+  </si>
+  <si>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>任职</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.235712508412994</v>
+        <v>0.261756970541316</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -494,7 +494,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.156993029575974</v>
+        <v>0.174339580426122</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -505,7 +505,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>0.137632257708554</v>
+        <v>0.152839588654459</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -516,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0.116456044376483</v>
+        <v>0.129323562769115</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -527,7 +527,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.110040921336493</v>
+        <v>0.122199616806708</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -538,7 +538,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>0.104156464239715</v>
+        <v>0.105768334142884</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -549,7 +549,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0.095244528922861</v>
+        <v>0.0744094388538612</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -560,7 +560,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>0.0720347976322613</v>
+        <v>0.0725960352426972</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -571,7 +571,7 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>0.0712947350969863</v>
+        <v>0.070042580339844</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -582,7 +582,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>0.0670058010129611</v>
+        <v>0.0694139430530066</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -593,7 +593,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>0.0653728285917542</v>
+        <v>0.0661276099031103</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -604,7 +604,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>0.063073438974636</v>
+        <v>0.0652240897031835</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -615,7 +615,7 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>0.062507350241809</v>
+        <v>0.0599854299557824</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -626,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>0.0595480027652513</v>
+        <v>0.0573462361267485</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -637,7 +637,7 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>0.0587343815948728</v>
+        <v>0.0540339004938619</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -648,7 +648,7 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>0.0540169613587336</v>
+        <v>0.0531218941676708</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -659,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>0.0537178555456348</v>
+        <v>0.0515685664314385</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -670,7 +670,7 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>0.0516403637218371</v>
+        <v>0.0487920824017798</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -681,7 +681,7 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>0.0486576009739385</v>
+        <v>0.0440095558918557</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -692,7 +692,7 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>0.0478363380353032</v>
+        <v>0.0425923943293341</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -703,7 +703,7 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>0.0471559594387298</v>
+        <v>0.0408008927865718</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -714,7 +714,7 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>0.0464375642936236</v>
+        <v>0.040127239673617</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -725,7 +725,7 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>0.0439373366441132</v>
+        <v>0.0393481806825429</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -736,7 +736,7 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>0.0396306650094493</v>
+        <v>0.0382079466474276</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -747,7 +747,7 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>0.0383545090926168</v>
+        <v>0.0376833239386981</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -758,7 +758,7 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>0.0367412595138302</v>
+        <v>0.036262559575537</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -769,7 +769,7 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <v>0.0361346339682853</v>
+        <v>0.0361490326800581</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -780,7 +780,7 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <v>0.0354330902859603</v>
+        <v>0.0361250523559445</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -791,7 +791,7 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>0.0344063079846559</v>
+        <v>0.0350599773257541</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -802,7 +802,7 @@
         <v>29</v>
       </c>
       <c r="C31">
-        <v>0.0339338845210541</v>
+        <v>0.0345023314386803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>